<commit_message>
Add some changes to the expense order xlsx file
</commit_message>
<xml_diff>
--- a/project/main/xlsx_files/expense_order.xlsx
+++ b/project/main/xlsx_files/expense_order.xlsx
@@ -258,7 +258,7 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="14" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="14" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -915,7 +915,7 @@
         <f>G3</f>
         <v/>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="13"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -28529,14 +28529,15 @@
       <c r="Z1000" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D5:F5"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="E13:I13"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B15:C15"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.0" footer="0.0" header="0.0" left="0.0" right="0.0" top="0.0"/>

</xml_diff>